<commit_message>
cambie formato de la plantilla
</commit_message>
<xml_diff>
--- a/public/doc/Plantilla_BaseDatos.xlsx
+++ b/public/doc/Plantilla_BaseDatos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS01\Documents\crearformato\public\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS01\Documents\crearFormato\client\public\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2E38BC-9BE6-479F-A90D-A367E485FF9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0644FF21-B634-4E76-A4B4-979CAA621DF7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>nombre</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>credencial</t>
+  </si>
+  <si>
+    <t>imagen</t>
   </si>
 </sst>
 </file>
@@ -331,10 +334,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -345,7 +348,7 @@
     <col min="5" max="5" width="12.6640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -370,20 +373,23 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E2"/>
     </row>
-    <row r="3" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E4"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E5"/>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E6"/>
     </row>
   </sheetData>

</xml_diff>